<commit_message>
cap nhat thang 12
</commit_message>
<xml_diff>
--- a/Level.xlsx
+++ b/Level.xlsx
@@ -63,9 +63,6 @@
     <t>Việc phân cấp ra các cấp độ sẽ cho ta biết ta đang ở đâu và cần làm gì để tiến lên một cấp độ cao hơn</t>
   </si>
   <si>
-    <t>Một người tham gia nhiều năm trong thị trường cũng chưa chắc đánh mà đem lại lợi nhuận nhiều như người mới tham gia được một hai năm, đó là phụ thuộc vào trình độ cũng như khả năng của mỗi người</t>
-  </si>
-  <si>
     <t>Cũng giống như luyện võ trong mấy bộ phim cổ trang</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>Khi hoàn thành những mục tiêu cho level này thì chúng ta sẽ tiến đến thực hiện level tiếp theo</t>
   </si>
   <si>
-    <t>Các cấp độ level phải có sự rõ ràng để khi hoàn thành những level dưới một cách thành thục thì mới có thể tăng cường cảnh giới đi đến thực hiện level tiếp theo</t>
-  </si>
-  <si>
     <t>Một người có thể xây dựng cho mình vài bộ level cùng lúc để có thể tăng cường trình độ cho mình</t>
   </si>
   <si>
@@ -343,6 +337,12 @@
   </si>
   <si>
     <t>Thi chuyển level</t>
+  </si>
+  <si>
+    <t>Một người tham gia nhiều năm trong thị trường cũng chưa chắc đánh mà đem lại lợi nhuận nhiều như người mới tham gia được một hai năm, đó là phụ thuộc vào khả năng giác ngộ của mỗi người</t>
+  </si>
+  <si>
+    <t>Các cấp độ level phải có sự phân cấp rõ ràng để khi hoàn thành những level dưới một cách thành thục thì mới có thể tăng cường cảnh giới đi đến thực hiện level tiếp theo</t>
   </si>
 </sst>
 </file>
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
@@ -1040,62 +1040,62 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
@@ -1104,19 +1104,19 @@
     <row r="36" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B36" s="8"/>
       <c r="C36" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" t="s">
+        <v>52</v>
+      </c>
+      <c r="L36" t="s">
         <v>53</v>
       </c>
-      <c r="F36" t="s">
-        <v>70</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="O36" t="s">
         <v>54</v>
-      </c>
-      <c r="L36" t="s">
-        <v>55</v>
-      </c>
-      <c r="O36" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="37" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
@@ -1125,15 +1125,15 @@
     <row r="38" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B38" s="8"/>
       <c r="C38" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D38" s="10"/>
       <c r="F38" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G38" s="12"/>
       <c r="I38" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J38" s="14"/>
       <c r="L38" s="37"/>
@@ -1143,553 +1143,553 @@
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C39" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D39" s="16"/>
       <c r="F39" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G39" s="21"/>
       <c r="I39" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J39" s="26"/>
       <c r="L39" s="39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M39" s="40"/>
       <c r="O39" s="32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P39" s="33"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C40" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I40" s="27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J40" s="26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L40" s="41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M40" s="40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O40" s="34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P40" s="33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C41" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G41" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I41" s="27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J41" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L41" s="41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M41" s="40" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O41" s="34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P41" s="33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C42" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F42" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I42" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J42" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L42" s="41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M42" s="40" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O42" s="34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P42" s="33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C43" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D43" s="16"/>
       <c r="F43" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G43" s="21"/>
       <c r="I43" s="27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J43" s="26"/>
       <c r="L43" s="41" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M43" s="40"/>
       <c r="O43" s="34" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P43" s="33"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C44" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D44" s="16"/>
       <c r="F44" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G44" s="21"/>
       <c r="I44" s="25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J44" s="26"/>
       <c r="L44" s="39" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M44" s="40"/>
       <c r="O44" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="P44" s="33"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C45" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F45" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G45" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I45" s="27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J45" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L45" s="41" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M45" s="40" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O45" s="34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P45" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C46" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I46" s="27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J46" s="26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L46" s="41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M46" s="40" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O46" s="34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P46" s="33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C47" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I47" s="28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J47" s="29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L47" s="42" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M47" s="43" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O47" s="35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P47" s="36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D49" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D56" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D61" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D64" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D66" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D68" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F80" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F81" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F82" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F83" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F84" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F85" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F86" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F87" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F88" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F89" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F90" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="94" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B94" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C95" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D96" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D97" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D98" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D99" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C100" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D100" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D101" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C103" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>